<commit_message>
11:38 - 31.01.2025 - Excel update
</commit_message>
<xml_diff>
--- a/NachDurchlaufplan/excelFiles/3-WD&DataHandling.xlsx
+++ b/NachDurchlaufplan/excelFiles/3-WD&DataHandling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/pit5lo_bosch_com/Documents/Ausbildung - Fachinformatik/NachDurchlaufplan/excelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="13_ncr:1_{FE1FF163-F8EE-4837-A48A-89B378637BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85D991F-FBAD-4C55-B467-C3052739B6A9}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{0407CCC0-2C79-44B3-8CC9-F13173F4F2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5816D424-7BEE-4763-9FAB-36DC9E9CA535}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="15615" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Time</t>
   </si>
@@ -132,6 +132,64 @@
   </si>
   <si>
     <t>1.1. Index</t>
+  </si>
+  <si>
+    <t>1. INDIVIDUAL CRUD</t>
+  </si>
+  <si>
+    <t>DB and Users' table</t>
+  </si>
+  <si>
+    <t>Connection to DB</t>
+  </si>
+  <si>
+    <t>Login and Register forms that save the inputs into PHP</t>
+  </si>
+  <si>
+    <t>Insert the variables stored in PHP, into the users table</t>
+  </si>
+  <si>
+    <t>Create very basic landing pages for clients and admins</t>
+  </si>
+  <si>
+    <t>Add a logout button</t>
+  </si>
+  <si>
+    <t>Create a table for products and purchases, with foreign keys</t>
+  </si>
+  <si>
+    <t>Add a form for owners to add products</t>
+  </si>
+  <si>
+    <t>Let the owners change the state of their products</t>
+  </si>
+  <si>
+    <t>Let the clients buy products</t>
+  </si>
+  <si>
+    <t>Landing page with a menu</t>
+  </si>
+  <si>
+    <t>Logout button</t>
+  </si>
+  <si>
+    <t>Create chats table and let users create those</t>
+  </si>
+  <si>
+    <t>Make a page for users to see all chats</t>
+  </si>
+  <si>
+    <t>Add to the landing page a table with chats they are part of</t>
+  </si>
+  <si>
+    <t>Add a table to the DB with chat participants, and functionality to join</t>
+  </si>
+  <si>
+    <t>Add a messages table to the DB, and functionality to insert messages to the chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect users based on their type
+</t>
   </si>
 </sst>
 </file>
@@ -195,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -774,17 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -813,26 +860,6 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -891,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -962,12 +989,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -986,244 +1091,139 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1277,6 +1277,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1729,37 +1733,37 @@
       <c r="A17" s="12">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
@@ -1821,11 +1825,11 @@
       <c r="A29" s="13">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1842,7 +1846,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B17"/>
+      <selection activeCell="B9" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,24 +1862,24 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="18"/>
@@ -1884,86 +1888,86 @@
       <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="78"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="47" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="48"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="43"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="68" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3"/>
@@ -1972,18 +1976,18 @@
       <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="70" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="21"/>
@@ -1992,59 +1996,59 @@
       <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="72">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="90"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="78"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="82"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="82"/>
+      <c r="A20" s="74"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="86"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="84"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="64" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="22"/>
@@ -2054,8 +2058,8 @@
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="78" t="s">
+      <c r="B23" s="59"/>
+      <c r="C23" s="62" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="3"/>
@@ -2064,54 +2068,59 @@
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="78"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="78"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="78"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="83"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="87"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B22:B28"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
@@ -2119,11 +2128,6 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B22:B28"/>
     <mergeCell ref="B9:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,198 +2155,198 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="93"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="98" t="s">
+      <c r="B6" s="98"/>
+      <c r="C6" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="97"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="97"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="97"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="98" t="s">
+      <c r="B9" s="98"/>
+      <c r="C9" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="97"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="108"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="97"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="102"/>
-      <c r="C13" s="98" t="s">
+      <c r="B13" s="95"/>
+      <c r="C13" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="111"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="109"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="102"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="103"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="106"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="70" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="18"/>
@@ -2351,24 +2355,24 @@
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="46"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="45" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="93" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="21"/>
@@ -2377,16 +2381,16 @@
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="46"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="92"/>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="45" t="s">
+      <c r="B27" s="88"/>
+      <c r="C27" s="93" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="21"/>
@@ -2395,35 +2399,35 @@
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="65"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B15:B17"/>
     <mergeCell ref="B22:B29"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2435,7 +2439,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D21"/>
+      <selection activeCell="B2" sqref="B2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,240 +2455,271 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="54"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="54"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="54"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="54"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="54"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="54"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="54"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="54"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="54"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="54"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="11">
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C9:C13"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2694,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A8BCDC-E960-4C7B-9139-1CC3BC203676}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,241 +2746,271 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="54"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="54"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="54"/>
-    </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="54"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="54"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="54"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="54"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="54"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="54"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="54"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="11">
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2956,7 +3021,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,246 +3037,261 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="68"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
+      <c r="C22" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="68"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="68"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B2:D17"/>
-    <mergeCell ref="B22:D29"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
14:25 - 04.02.2025 - 3rd week in 0 excel finished
</commit_message>
<xml_diff>
--- a/NachDurchlaufplan/excelFiles/3-WD&DataHandling.xlsx
+++ b/NachDurchlaufplan/excelFiles/3-WD&DataHandling.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/pit5lo_bosch_com/Documents/Ausbildung - Fachinformatik/NachDurchlaufplan/excelFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="313" documentId="13_ncr:1_{FE1FF163-F8EE-4837-A48A-89B378637BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B85D991F-FBAD-4C55-B467-C3052739B6A9}"/>
+  <xr:revisionPtr revIDLastSave="185" documentId="8_{0407CCC0-2C79-44B3-8CC9-F13173F4F2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5816D424-7BEE-4763-9FAB-36DC9E9CA535}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="15615" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{9CD730A3-8F49-4384-BBDD-74FD70423D42}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="2" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="47">
   <si>
     <t>Time</t>
   </si>
@@ -132,6 +132,64 @@
   </si>
   <si>
     <t>1.1. Index</t>
+  </si>
+  <si>
+    <t>1. INDIVIDUAL CRUD</t>
+  </si>
+  <si>
+    <t>DB and Users' table</t>
+  </si>
+  <si>
+    <t>Connection to DB</t>
+  </si>
+  <si>
+    <t>Login and Register forms that save the inputs into PHP</t>
+  </si>
+  <si>
+    <t>Insert the variables stored in PHP, into the users table</t>
+  </si>
+  <si>
+    <t>Create very basic landing pages for clients and admins</t>
+  </si>
+  <si>
+    <t>Add a logout button</t>
+  </si>
+  <si>
+    <t>Create a table for products and purchases, with foreign keys</t>
+  </si>
+  <si>
+    <t>Add a form for owners to add products</t>
+  </si>
+  <si>
+    <t>Let the owners change the state of their products</t>
+  </si>
+  <si>
+    <t>Let the clients buy products</t>
+  </si>
+  <si>
+    <t>Landing page with a menu</t>
+  </si>
+  <si>
+    <t>Logout button</t>
+  </si>
+  <si>
+    <t>Create chats table and let users create those</t>
+  </si>
+  <si>
+    <t>Make a page for users to see all chats</t>
+  </si>
+  <si>
+    <t>Add to the landing page a table with chats they are part of</t>
+  </si>
+  <si>
+    <t>Add a table to the DB with chat participants, and functionality to join</t>
+  </si>
+  <si>
+    <t>Add a messages table to the DB, and functionality to insert messages to the chat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Redirect users based on their type
+</t>
   </si>
 </sst>
 </file>
@@ -195,7 +253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="52">
     <border>
       <left/>
       <right/>
@@ -774,17 +832,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -813,26 +860,6 @@
       </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -891,7 +918,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="112">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -962,12 +989,90 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="50" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -986,244 +1091,139 @@
     <xf numFmtId="165" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1277,6 +1277,10 @@
     </sheetDataSet>
   </externalBook>
 </externalLink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1729,37 +1733,37 @@
       <c r="A17" s="12">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="64"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="16"/>
       <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12">
@@ -1821,11 +1825,11 @@
       <c r="A29" s="13">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1842,7 +1846,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B17"/>
+      <selection activeCell="B9" sqref="B9:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,24 +1862,24 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="61" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="18"/>
@@ -1884,86 +1888,86 @@
       <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="78"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="78"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="40"/>
-      <c r="C5" s="83"/>
-      <c r="D5" s="19"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="40"/>
-      <c r="C6" s="47" t="s">
+      <c r="B6" s="59"/>
+      <c r="C6" s="62" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="18"/>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="40"/>
-      <c r="C7" s="41"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="39"/>
-      <c r="C8" s="48"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="63"/>
       <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="91" t="s">
+      <c r="C9" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="21"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="50"/>
-      <c r="C10" s="43"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="50"/>
-      <c r="C11" s="92"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="50"/>
-      <c r="C12" s="42" t="s">
+      <c r="B12" s="59"/>
+      <c r="C12" s="68" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="3"/>
@@ -1972,18 +1976,18 @@
       <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="44"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="69"/>
       <c r="D13" s="19"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="47" t="s">
+      <c r="C14" s="70" t="s">
         <v>10</v>
       </c>
       <c r="D14" s="21"/>
@@ -1992,59 +1996,59 @@
       <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="41"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="71"/>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="41"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="71"/>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="53"/>
-      <c r="C17" s="48"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="72"/>
       <c r="D17" s="17"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="72">
+      <c r="A18" s="73">
         <v>0.5</v>
       </c>
-      <c r="B18" s="88" t="s">
+      <c r="B18" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="89"/>
-      <c r="D18" s="90"/>
+      <c r="C18" s="77"/>
+      <c r="D18" s="78"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="73"/>
-      <c r="B19" s="81"/>
-      <c r="C19" s="79"/>
-      <c r="D19" s="82"/>
+      <c r="A19" s="74"/>
+      <c r="B19" s="79"/>
+      <c r="C19" s="80"/>
+      <c r="D19" s="81"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="73"/>
-      <c r="B20" s="81"/>
-      <c r="C20" s="79"/>
-      <c r="D20" s="82"/>
+      <c r="A20" s="74"/>
+      <c r="B20" s="79"/>
+      <c r="C20" s="80"/>
+      <c r="D20" s="81"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="74"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="85"/>
-      <c r="D21" s="86"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="82"/>
+      <c r="C21" s="83"/>
+      <c r="D21" s="84"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="64" t="s">
         <v>9</v>
       </c>
       <c r="C22" s="22"/>
@@ -2054,8 +2058,8 @@
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="50"/>
-      <c r="C23" s="78" t="s">
+      <c r="B23" s="59"/>
+      <c r="C23" s="62" t="s">
         <v>11</v>
       </c>
       <c r="D23" s="3"/>
@@ -2064,54 +2068,59 @@
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="50"/>
-      <c r="C24" s="78"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="50"/>
-      <c r="C25" s="78"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="50"/>
-      <c r="C26" s="78"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="50"/>
-      <c r="C27" s="78"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="51"/>
-      <c r="C28" s="83"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="63"/>
       <c r="D28" s="19"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="39" t="s">
+      <c r="B29" s="85" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="87"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C23:C28"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B22:B28"/>
     <mergeCell ref="B14:B17"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
@@ -2119,11 +2128,6 @@
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C17"/>
-    <mergeCell ref="C23:C28"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B22:B28"/>
     <mergeCell ref="B9:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2151,198 +2155,198 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="76" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="77" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="71">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="100" t="s">
+      <c r="C2" s="101" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="93"/>
+      <c r="D2" s="32"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="101"/>
-      <c r="C3" s="98"/>
-      <c r="D3" s="97"/>
+      <c r="B3" s="98"/>
+      <c r="C3" s="90"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="101"/>
-      <c r="C4" s="98"/>
-      <c r="D4" s="97"/>
+      <c r="B4" s="98"/>
+      <c r="C4" s="90"/>
+      <c r="D4" s="33"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="101"/>
-      <c r="C5" s="98"/>
-      <c r="D5" s="97"/>
+      <c r="B5" s="98"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="33"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="101"/>
-      <c r="C6" s="98" t="s">
+      <c r="B6" s="98"/>
+      <c r="C6" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="97"/>
+      <c r="D6" s="33"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="101"/>
-      <c r="C7" s="98"/>
-      <c r="D7" s="97"/>
+      <c r="B7" s="98"/>
+      <c r="C7" s="90"/>
+      <c r="D7" s="33"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="101"/>
-      <c r="C8" s="98"/>
-      <c r="D8" s="97"/>
+      <c r="B8" s="98"/>
+      <c r="C8" s="90"/>
+      <c r="D8" s="33"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="101"/>
-      <c r="C9" s="98" t="s">
+      <c r="B9" s="98"/>
+      <c r="C9" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="97"/>
+      <c r="D9" s="33"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="107"/>
-      <c r="C10" s="95"/>
-      <c r="D10" s="108"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="110" t="s">
+      <c r="B11" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="100" t="s">
+      <c r="C11" s="101" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="93"/>
+      <c r="D11" s="32"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="102"/>
-      <c r="C12" s="98"/>
-      <c r="D12" s="97"/>
+      <c r="B12" s="95"/>
+      <c r="C12" s="90"/>
+      <c r="D12" s="33"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="102"/>
-      <c r="C13" s="98" t="s">
+      <c r="B13" s="95"/>
+      <c r="C13" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="97"/>
+      <c r="D13" s="33"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="104"/>
-      <c r="C14" s="105"/>
-      <c r="D14" s="111"/>
+      <c r="B14" s="96"/>
+      <c r="C14" s="91"/>
+      <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="96" t="s">
+      <c r="B15" s="100" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="94" t="s">
+      <c r="C15" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="109"/>
+      <c r="D15" s="37"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="102"/>
-      <c r="C16" s="98"/>
-      <c r="D16" s="103"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="34"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="104"/>
-      <c r="C17" s="105"/>
-      <c r="D17" s="106"/>
+      <c r="B17" s="96"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="35"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="25"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="70" t="s">
         <v>21</v>
       </c>
       <c r="D22" s="18"/>
@@ -2351,24 +2355,24 @@
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="40"/>
-      <c r="C23" s="41"/>
+      <c r="B23" s="88"/>
+      <c r="C23" s="71"/>
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="40"/>
-      <c r="C24" s="46"/>
+      <c r="B24" s="88"/>
+      <c r="C24" s="92"/>
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="45" t="s">
+      <c r="B25" s="88"/>
+      <c r="C25" s="93" t="s">
         <v>22</v>
       </c>
       <c r="D25" s="21"/>
@@ -2377,16 +2381,16 @@
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="40"/>
-      <c r="C26" s="46"/>
+      <c r="B26" s="88"/>
+      <c r="C26" s="92"/>
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="40"/>
-      <c r="C27" s="45" t="s">
+      <c r="B27" s="88"/>
+      <c r="C27" s="93" t="s">
         <v>23</v>
       </c>
       <c r="D27" s="21"/>
@@ -2395,35 +2399,35 @@
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="40"/>
-      <c r="C28" s="41"/>
+      <c r="B28" s="88"/>
+      <c r="C28" s="71"/>
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="75">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="39"/>
-      <c r="C29" s="48"/>
-      <c r="D29" s="65"/>
+      <c r="B29" s="85"/>
+      <c r="C29" s="72"/>
+      <c r="D29" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B15:B17"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="C6:C8"/>
     <mergeCell ref="C9:C10"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="B11:B14"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="B15:B17"/>
     <mergeCell ref="B22:B29"/>
     <mergeCell ref="C15:C17"/>
     <mergeCell ref="C22:C24"/>
     <mergeCell ref="C25:C26"/>
     <mergeCell ref="C27:C29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="B18:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2435,7 +2439,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18:D21"/>
+      <selection activeCell="B2" sqref="B2:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2451,240 +2455,271 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="54"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="54"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="54"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="54"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="54"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="54"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="45"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="49"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="54"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62" t="s">
+        <v>35</v>
+      </c>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="54"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="54"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="54"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="11">
+    <mergeCell ref="C27:C29"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C9:C13"/>
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="C22:C23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2694,8 +2729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44A8BCDC-E960-4C7B-9139-1CC3BC203676}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2711,241 +2746,271 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="54"/>
+      <c r="B2" s="64" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="54"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="54"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="54"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="54"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="54"/>
-    </row>
-    <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="B8" s="59"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="54"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="17"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="54"/>
+      <c r="B10" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="39"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="54"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="54"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="54"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="54"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="54"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="54"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="56"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="54"/>
+      <c r="B22" s="64" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="54"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="54"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="54"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="54"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="54"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="54"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="54"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="11">
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B2:B9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="C26:C29"/>
+    <mergeCell ref="C23:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2956,7 +3021,7 @@
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2972,246 +3037,261 @@
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11">
+      <c r="A2" s="26">
         <v>0.33333333333333331</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="A3" s="20">
         <v>0.34375</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="68"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="40"/>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="A4" s="20">
         <v>0.35416666666666702</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="68"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="40"/>
     </row>
     <row r="5" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
+      <c r="A5" s="20">
         <v>0.36458333333333298</v>
       </c>
-      <c r="B5" s="66"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="68"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="40"/>
     </row>
     <row r="6" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
+      <c r="A6" s="20">
         <v>0.375</v>
       </c>
-      <c r="B6" s="66"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="68"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="40"/>
     </row>
     <row r="7" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
+      <c r="A7" s="20">
         <v>0.38541666666666702</v>
       </c>
-      <c r="B7" s="66"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="68"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="40"/>
     </row>
     <row r="8" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
+      <c r="A8" s="20">
         <v>0.39583333333333298</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="68"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="40"/>
     </row>
     <row r="9" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
+      <c r="A9" s="20">
         <v>0.40625</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="68"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="40"/>
     </row>
     <row r="10" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
+      <c r="A10" s="20">
         <v>0.41666666666666702</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="68"/>
+      <c r="B10" s="59"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="40"/>
     </row>
     <row r="11" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
+      <c r="A11" s="20">
         <v>0.42708333333333298</v>
       </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="68"/>
+      <c r="B11" s="59"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="40"/>
     </row>
     <row r="12" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
+      <c r="A12" s="20">
         <v>0.4375</v>
       </c>
-      <c r="B12" s="66"/>
-      <c r="C12" s="67"/>
-      <c r="D12" s="68"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="40"/>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12">
+      <c r="A13" s="20">
         <v>0.44791666666666702</v>
       </c>
-      <c r="B13" s="66"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="68"/>
+      <c r="B13" s="59"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12">
+      <c r="A14" s="20">
         <v>0.45833333333333298</v>
       </c>
-      <c r="B14" s="66"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="B14" s="59"/>
+      <c r="C14" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="40"/>
     </row>
     <row r="15" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
+      <c r="A15" s="20">
         <v>0.46875</v>
       </c>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="68"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="40"/>
     </row>
     <row r="16" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
+      <c r="A16" s="20">
         <v>0.47916666666666702</v>
       </c>
-      <c r="B16" s="66"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="68"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="40"/>
     </row>
     <row r="17" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="12">
+      <c r="A17" s="20">
         <v>0.48958333333333298</v>
       </c>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="37"/>
+      <c r="B17" s="65"/>
+      <c r="C17" s="63"/>
+      <c r="D17" s="42"/>
     </row>
     <row r="18" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="29">
+      <c r="A18" s="55">
         <v>0.5</v>
       </c>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
-      <c r="D18" s="59"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
     </row>
     <row r="19" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="46"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
     </row>
     <row r="20" spans="1:4" ht="6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+      <c r="A20" s="56"/>
+      <c r="B20" s="46"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
     </row>
     <row r="21" spans="1:4" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="31"/>
-      <c r="B21" s="61"/>
-      <c r="C21" s="62"/>
-      <c r="D21" s="63"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="48"/>
     </row>
     <row r="22" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="20">
         <v>0.54166666666666696</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
+      <c r="C22" s="61" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="20">
         <v>0.55208333333333304</v>
       </c>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="68"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="62"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="20">
         <v>0.5625</v>
       </c>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="68"/>
+      <c r="B24" s="59"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="40"/>
     </row>
     <row r="25" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="20">
         <v>0.57291666666666696</v>
       </c>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="68"/>
+      <c r="B25" s="59"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="20">
         <v>0.58333333333333304</v>
       </c>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="68"/>
+      <c r="B26" s="59"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="40"/>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20">
         <v>0.59375</v>
       </c>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="68"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20">
         <v>0.60416666666666696</v>
       </c>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="68"/>
+      <c r="B28" s="59"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="40"/>
     </row>
     <row r="29" spans="1:4" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="13">
+      <c r="A29" s="27">
         <v>0.61458333333333304</v>
       </c>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="70"/>
+      <c r="B29" s="65"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="42"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="9">
     <mergeCell ref="A18:A21"/>
     <mergeCell ref="B18:D21"/>
-    <mergeCell ref="B2:D17"/>
-    <mergeCell ref="B22:D29"/>
+    <mergeCell ref="B2:B17"/>
+    <mergeCell ref="B22:B29"/>
+    <mergeCell ref="C22:C29"/>
+    <mergeCell ref="C14:C17"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="C4:C7"/>
+    <mergeCell ref="C2:C3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>